<commit_message>
getter data excel list
</commit_message>
<xml_diff>
--- a/res/hospital_list_test.xlsx
+++ b/res/hospital_list_test.xlsx
@@ -486,10 +486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A38"/>
+  <dimension ref="A2:B39"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -497,189 +497,306 @@
     <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B5">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B6">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B8">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B11">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B13">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B15">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B16">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B18">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B20">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B21">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B28">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B29">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B31">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B34">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>36</v>
+      </c>
+      <c r="B38">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B39">
+        <f>SUM(B2:B38)</f>
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Hospitals fix + expected hat fix
</commit_message>
<xml_diff>
--- a/res/hospital_list_test.xlsx
+++ b/res/hospital_list_test.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\לימודים\שנה ד\OneSideMatching\res\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F7A47E-F147-4D33-869F-D141D99B974F}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="75" windowWidth="20400" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="75" windowWidth="20400" windowHeight="7995" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
     <sheet name="גיליון2" sheetId="2" r:id="rId2"/>
     <sheet name="גיליון3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -132,20 +138,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="177"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="177"/>
@@ -176,24 +173,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="היפר-קישור" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -242,7 +240,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -275,9 +273,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -310,6 +325,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -485,11 +517,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B39"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:B40"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -497,344 +529,313 @@
     <col min="1" max="1" width="27.25" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>23</v>
-      </c>
-    </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>3</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10">
-        <v>32</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13">
-        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
-        <v>32</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
+      <c r="B17">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A17" s="1" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B17">
+      <c r="B18">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B19">
         <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B21">
+      <c r="B22">
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A22" s="1" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B22">
+      <c r="B23">
         <v>7</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A23" s="1" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B23">
+      <c r="B24">
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A24" s="1" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B24">
+      <c r="B25">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A25" s="1" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B25">
+      <c r="B26">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A26" s="1" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B26">
+      <c r="B27">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A27" s="1" t="s">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B27">
+      <c r="B28">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A28" s="1" t="s">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B28">
+      <c r="B29">
         <v>12</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A29" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B29">
-        <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A32" s="1" t="s">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B32">
+      <c r="B33">
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A33" s="1" t="s">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B33">
+      <c r="B34">
         <v>13</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A34" s="1" t="s">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B34">
+      <c r="B35">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B35">
+      <c r="B36">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A36" s="1" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="B36">
+      <c r="B37">
         <v>12</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B37">
-        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B38">
+      <c r="B39">
         <v>7</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="B39">
-        <f>SUM(B2:B38)</f>
-        <v>500</v>
-      </c>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" tooltip="Yitzhak Shamir Medical Center" display="https://en.wikipedia.org/wiki/Yitzhak_Shamir_Medical_Center"/>
-    <hyperlink ref="A5" r:id="rId2" tooltip="Kiryat Shlomo" display="https://en.wikipedia.org/wiki/Kiryat_Shlomo"/>
-    <hyperlink ref="A6" r:id="rId3" tooltip="Meir Hospital" display="https://en.wikipedia.org/wiki/Meir_Hospital"/>
-    <hyperlink ref="A9" r:id="rId4" tooltip="Laniado Hospital" display="https://en.wikipedia.org/wiki/Laniado_Hospital"/>
-    <hyperlink ref="A11" r:id="rId5" tooltip="Rabin Medical Center" display="https://en.wikipedia.org/wiki/Rabin_Medical_Center"/>
-    <hyperlink ref="A14" r:id="rId6" tooltip="Kaplan Medical Center" display="https://en.wikipedia.org/wiki/Kaplan_Medical_Center"/>
-    <hyperlink ref="A16" r:id="rId7" tooltip="Hillel Yaffe Medical Center" display="https://en.wikipedia.org/wiki/Hillel_Yaffe_Medical_Center"/>
-    <hyperlink ref="A17" r:id="rId8" tooltip="Bnai Zion Medical Center" display="https://en.wikipedia.org/wiki/Bnai_Zion_Medical_Center"/>
-    <hyperlink ref="A18" r:id="rId9" tooltip="Carmel Hospital (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Carmel_Hospital&amp;action=edit&amp;redlink=1"/>
-    <hyperlink ref="A19" r:id="rId10" tooltip="Rambam Health Care Campus" display="https://en.wikipedia.org/wiki/Rambam_Health_Care_Campus"/>
-    <hyperlink ref="A21" r:id="rId11" tooltip="Bikur Holim Hospital" display="https://en.wikipedia.org/wiki/Bikur_Holim_Hospital"/>
-    <hyperlink ref="A22" r:id="rId12" location="Ein_Kerem_campus" tooltip="Hadassah Medical Center" display="https://en.wikipedia.org/wiki/Hadassah_Medical_Center - Ein_Kerem_campus"/>
-    <hyperlink ref="A23" r:id="rId13" location="Mount_Scopus_campus" tooltip="Hadassah Medical Center" display="https://en.wikipedia.org/wiki/Hadassah_Medical_Center - Mount_Scopus_campus"/>
-    <hyperlink ref="A24" r:id="rId14" tooltip="Augusta Victoria Hospital" display="https://en.wikipedia.org/wiki/Augusta_Victoria_Hospital"/>
-    <hyperlink ref="A25" r:id="rId15" tooltip="Al-Makassed Islamic Charitable Hospital" display="https://en.wikipedia.org/wiki/Al-Makassed_Islamic_Charitable_Hospital"/>
-    <hyperlink ref="A26" r:id="rId16" tooltip="HaEmek Medical Center" display="https://en.wikipedia.org/wiki/HaEmek_Medical_Center"/>
-    <hyperlink ref="A27" r:id="rId17" tooltip="Baruch Padeh Medical Center" display="https://en.wikipedia.org/wiki/Baruch_Padeh_Medical_Center"/>
-    <hyperlink ref="A28" r:id="rId18" tooltip="Galilee Medical Center" display="https://en.wikipedia.org/wiki/Galilee_Medical_Center"/>
-    <hyperlink ref="A29" r:id="rId19" tooltip="EMMS Nazareth Hospital" display="https://en.wikipedia.org/wiki/EMMS_Nazareth_Hospital"/>
-    <hyperlink ref="A31" r:id="rId20" tooltip="Rebecca Sieff Hospital" display="https://en.wikipedia.org/wiki/Rebecca_Sieff_Hospital"/>
-    <hyperlink ref="A32" r:id="rId21" tooltip="Assuta Ashdod Medical Center" display="https://en.wikipedia.org/wiki/Assuta_Ashdod_Medical_Center"/>
-    <hyperlink ref="A33" r:id="rId22" tooltip="Barzilai Medical Center" display="https://en.wikipedia.org/wiki/Barzilai_Medical_Center"/>
-    <hyperlink ref="A34" r:id="rId23" tooltip="Soroka Medical Center" display="https://en.wikipedia.org/wiki/Soroka_Medical_Center"/>
-    <hyperlink ref="A35" r:id="rId24" tooltip="Yoseftal Medical Center" display="https://en.wikipedia.org/wiki/Yoseftal_Medical_Center"/>
-    <hyperlink ref="A36" r:id="rId25" tooltip="Ma'ayanei HaYeshua Hospital (page does not exist)" display="https://en.wikipedia.org/w/index.php?title=Ma%27ayanei_HaYeshua_Hospital&amp;action=edit&amp;redlink=1"/>
-    <hyperlink ref="A37" r:id="rId26" tooltip="Wolfson Medical Center" display="https://en.wikipedia.org/wiki/Wolfson_Medical_Center"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId27"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>
@@ -846,7 +847,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView rightToLeft="1" workbookViewId="0"/>

</xml_diff>